<commit_message>
Added logs page instead of user information
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t>Photograph</t>
   </si>
@@ -26,16 +26,25 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Назар Артемьев</t>
+  </si>
+  <si>
+    <t>HelliosSupport@gmail.com</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
     <t>Степан Третьяков</t>
   </si>
   <si>
-    <t>HelliosSupport@gmail.com</t>
+    <t>Павел Гелетей</t>
+  </si>
+  <si>
+    <t>Done.</t>
   </si>
   <si>
     <t>In progress.</t>
-  </si>
-  <si>
-    <t>Павел Гелетей</t>
   </si>
 </sst>
 </file>
@@ -80,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -122,7 +131,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>44511.0</v>
+        <v>44513.0</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -130,16 +139,86 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>44504.0</v>
+        <v>44501.0</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>44518.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>44513.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>44513.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>44513.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>44513.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>